<commit_message>
improved ui for first task
</commit_message>
<xml_diff>
--- a/Backend/AIBackend/outputs/ak956901@gmail.com/extracted_metadata.xlsx
+++ b/Backend/AIBackend/outputs/ak956901@gmail.com/extracted_metadata.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,7 @@
     <col width="30" customWidth="1" min="4" max="4"/>
     <col width="30" customWidth="1" min="5" max="5"/>
     <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -495,6 +496,11 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
+          <t>BW2024-08</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
           <t>PN2024-14A</t>
         </is>
       </c>
@@ -521,6 +527,11 @@
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>Experion PKS</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
         <is>
           <t>Experion PKS</t>
         </is>
@@ -560,6 +571,14 @@
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
+          <t>Unit Operations Controller (UOC)
+Ethernet Interface Module (EIM)
+ELCN Bridge
+ELCN Node</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
           <t>Unified Data Collector (UDC) on Experion PKS
 C200/C300 controllers</t>
         </is>
@@ -573,7 +592,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>Firmware versions released before PAR 1-FM396Q5/REUCN-7883 are fixed.</t>
+          <t>Firmware versions released before PAR 1-FM396Q5/REUCN-7883 are fixed</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
@@ -592,6 +611,13 @@
       </c>
       <c r="F5" s="5" t="inlineStr">
         <is>
+          <t>R511.5 initial release to R511.5 TCU5 HF2
+R520.2 initial release to R520.2 TCU6 HF3
+R530 initial release</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
           <t>R150.1</t>
         </is>
       </c>
@@ -606,8 +632,7 @@
         <is>
           <t>Experion PKS R511.5 TCU6
 Experion PKS R520.2 TCU6 HF2
-Experion PKS R520.2 TCU7
-R520.2 TCU6 HF2 or greater</t>
+Experion PKS R520.2 TCU7</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
@@ -627,6 +652,13 @@
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
+          <t>Experion PKS R511.5 TCU6 (Q4, 2024)
+Experion PKS R520.2 TCU7 (Released)
+Experion PKS R530 TCU1 (Q4, 2024)</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
           <t>R150.2</t>
         </is>
       </c>
@@ -655,6 +687,11 @@
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
+          <t>1-G9ENCXT</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
           <t>LSSES-18670</t>
         </is>
       </c>
@@ -682,13 +719,18 @@
       </c>
       <c r="F8" s="5" t="inlineStr">
         <is>
-          <t>Experion PKS Servers containing C200/C300 controllers with UDC Controller Collection checked</t>
+          <t>Experion PKS customers using UOC, EIM, ELCN BRIDGE, or ELCN NODE</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>Experion PKS Servers with UDC Controller Collection checked and C200/C300 controllers</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>